<commit_message>
basic capsnet size reduction
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77DA8698-3C7C-4C24-8C94-1A04D9530D78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{06B40BF2-E764-4045-AEBE-FA0F52040F54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Experiment</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>0_background</t>
+  </si>
+  <si>
+    <t>1_voice</t>
+  </si>
+  <si>
+    <t>1_background</t>
+  </si>
+  <si>
+    <t>Unet trained on full chime and librispeech dataset (10 epochs)</t>
   </si>
 </sst>
 </file>
@@ -160,9 +169,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,14 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -655,7 +670,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -681,9 +696,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B10" s="1"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -704,10 +717,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>43367</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>50</v>
       </c>
       <c r="C11">
@@ -733,12 +746,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>43367</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -762,10 +771,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>43368</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -786,11 +795,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -809,8 +820,118 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43369</v>
+      </c>
+      <c r="B15" s="1">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15">
+        <v>5.8499455248008101E-3</v>
+      </c>
+      <c r="E15">
+        <v>-4.9414299214992896</v>
+      </c>
+      <c r="F15">
+        <v>-2.9187624359262498</v>
+      </c>
+      <c r="G15">
+        <v>8.0849444575939504</v>
+      </c>
+      <c r="H15">
+        <v>-6.4876311729494796E-4</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>5.8499455248008101E-3</v>
+      </c>
+      <c r="E16">
+        <v>0.603653156846512</v>
+      </c>
+      <c r="F16">
+        <v>4.9341611496209197</v>
+      </c>
+      <c r="G16">
+        <v>8.0871218884956892</v>
+      </c>
+      <c r="H16">
+        <v>1.54551858325779E-2</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>3.9196163864368798E-3</v>
+      </c>
+      <c r="E17">
+        <v>0.10210658794458299</v>
+      </c>
+      <c r="F17">
+        <v>6.2019812058338104</v>
+      </c>
+      <c r="G17">
+        <v>4.9962338577947696</v>
+      </c>
+      <c r="H17">
+        <v>5.0428877463265804</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18">
+        <v>3.9196163864368798E-3</v>
+      </c>
+      <c r="E18">
+        <v>4.17242882565266</v>
+      </c>
+      <c r="F18">
+        <v>13.924662842344301</v>
+      </c>
+      <c r="G18">
+        <v>5.65928442136721</v>
+      </c>
+      <c r="H18">
+        <v>3.58423085463872</v>
+      </c>
+      <c r="I18" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
config chg for re-test using only chime data
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{06B40BF2-E764-4045-AEBE-FA0F52040F54}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91C684C7-E064-4EDD-958F-A17BECBDF19D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>Experiment</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Unet trained on full chime and librispeech dataset (10 epochs)</t>
+  </si>
+  <si>
+    <t>Same Unet as 52, tested only on chime test-set</t>
   </si>
 </sst>
 </file>
@@ -491,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -532,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>36</v>
       </c>
@@ -558,7 +561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>37</v>
       </c>
@@ -584,7 +587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>37</v>
       </c>
@@ -607,7 +610,7 @@
         <v>4.5625503126689404</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>40</v>
       </c>
@@ -630,7 +633,7 @@
         <v>1.01601424866862E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>40</v>
       </c>
@@ -653,7 +656,7 @@
         <v>5.2170367078359199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>48</v>
       </c>
@@ -661,7 +664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>49</v>
       </c>
@@ -669,7 +672,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -695,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10">
         <v>1</v>
@@ -716,7 +719,7 @@
         <v>9.9428347412899996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43367</v>
       </c>
@@ -745,7 +748,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12">
@@ -770,7 +773,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43368</v>
       </c>
@@ -799,7 +802,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
@@ -822,7 +825,7 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43369</v>
       </c>
@@ -851,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" t="s">
@@ -874,7 +877,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" t="s">
@@ -897,7 +900,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" t="s">
@@ -920,17 +923,22 @@
       </c>
       <c r="I18" s="1"/>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -945,17 +953,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -963,7 +971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -971,42 +979,42 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Skip connections added to complex model
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5E4688B6-17AE-4C3D-BFA2-7A181989DD1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA0F7A43-5069-4E4B-AA86-B4F13AA2D1DC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Experiment</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>Same Unet as 52, tested only on chime test-set</t>
+  </si>
+  <si>
+    <t>Overtain test on small complex capsunet</t>
   </si>
 </sst>
 </file>
@@ -174,10 +177,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,19 +497,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -535,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>36</v>
       </c>
@@ -561,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>37</v>
       </c>
@@ -587,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>37</v>
       </c>
@@ -610,7 +613,7 @@
         <v>4.5625503126689404</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>40</v>
       </c>
@@ -633,7 +636,7 @@
         <v>1.01601424866862E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>40</v>
       </c>
@@ -656,7 +659,7 @@
         <v>5.2170367078359199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>48</v>
       </c>
@@ -664,7 +667,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>49</v>
       </c>
@@ -672,8 +675,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -698,8 +701,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -719,11 +722,11 @@
         <v>9.9428347412899996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>43367</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>50</v>
       </c>
       <c r="C11">
@@ -748,9 +751,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -773,11 +776,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>43368</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -798,13 +801,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -823,13 +826,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>43369</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>52</v>
       </c>
       <c r="C15" t="s">
@@ -850,13 +853,13 @@
       <c r="H15">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -875,11 +878,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
       <c r="C17" t="s">
         <v>33</v>
       </c>
@@ -898,11 +901,11 @@
       <c r="H17">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -921,13 +924,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>43370</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -948,13 +951,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -973,10 +976,111 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43373</v>
+      </c>
+      <c r="B21" s="1">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>0.147776272892951</v>
+      </c>
+      <c r="E21">
+        <v>5.6241614013729002</v>
+      </c>
+      <c r="F21">
+        <v>5.6760089425194096</v>
+      </c>
+      <c r="G21">
+        <v>26.4118842827855</v>
+      </c>
+      <c r="H21">
+        <v>8.5946525098830606E-3</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>0.147776272892951</v>
+      </c>
+      <c r="E22">
+        <v>14.036003919873201</v>
+      </c>
+      <c r="F22">
+        <v>14.3121284330277</v>
+      </c>
+      <c r="G22">
+        <v>26.441455970861998</v>
+      </c>
+      <c r="H22">
+        <v>3.6873848603017803E-2</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>0.12048309892416</v>
+      </c>
+      <c r="E23">
+        <v>6.4002952428711497</v>
+      </c>
+      <c r="F23">
+        <v>6.9678994223242396</v>
+      </c>
+      <c r="G23">
+        <v>17.126280309083199</v>
+      </c>
+      <c r="H23">
+        <v>0.78472849400813605</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24">
+        <v>0.12048309892416</v>
+      </c>
+      <c r="E24">
+        <v>14.019412077643</v>
+      </c>
+      <c r="F24">
+        <v>14.6675048806988</v>
+      </c>
+      <c r="G24">
+        <v>22.943669191124801</v>
+      </c>
+      <c r="H24">
+        <v>2.0282006372733901E-2</v>
+      </c>
+      <c r="I24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="I21:I24"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="A19:A20"/>
@@ -1003,17 +1107,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1029,42 +1133,42 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
config chg for mini test
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{15239F08-91A7-4749-BA39-78A4363614B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D3AAA5B6-74F5-43C8-88EF-6635FF2A046B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
   <si>
     <t>Experiment</t>
   </si>
@@ -142,10 +142,16 @@
     <t>Overtain test on small complex capsunet (no skip connections)</t>
   </si>
   <si>
-    <t>Running on Asia, small complex capsnet, no skips, full data, 10 epochs</t>
-  </si>
-  <si>
-    <t>Running on Europe small complex capsnet, with skips, full data, 10 epochs</t>
+    <t>Experiment with both GPUs, small complex capsnet, batch size=15, failed</t>
+  </si>
+  <si>
+    <t>Experiment with both GPUs, small complex capsnet, batch size=10, failed</t>
+  </si>
+  <si>
+    <t>Running on Asia, small complex capsnet, no skips, full data, 10 epochs, batch_size=5</t>
+  </si>
+  <si>
+    <t>Running on Europe small complex capsnet, with skips, full data, 10 epochs, batch_size=5</t>
   </si>
 </sst>
 </file>
@@ -183,13 +189,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +689,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -709,7 +715,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="B10" s="3"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -730,10 +736,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>43367</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>50</v>
       </c>
       <c r="C11">
@@ -759,8 +765,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -784,10 +790,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>43368</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -808,13 +814,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -833,13 +839,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>43369</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>52</v>
       </c>
       <c r="C15" t="s">
@@ -860,13 +866,13 @@
       <c r="H15">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -885,11 +891,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
       <c r="C17" t="s">
         <v>33</v>
       </c>
@@ -908,11 +914,11 @@
       <c r="H17">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -931,13 +937,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>43370</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -958,13 +964,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -983,13 +989,13 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>43373</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>61</v>
       </c>
       <c r="C21" t="s">
@@ -1010,13 +1016,13 @@
       <c r="H21">
         <v>8.5946525098830606E-3</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -1035,11 +1041,11 @@
       <c r="H22">
         <v>3.6873848603017803E-2</v>
       </c>
-      <c r="I22" s="2"/>
+      <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
@@ -1058,11 +1064,11 @@
       <c r="H23">
         <v>0.78472849400813605</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -1081,27 +1087,49 @@
       <c r="H24">
         <v>2.0282006372733901E-2</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="1">
         <v>43373</v>
       </c>
       <c r="B25">
         <v>64</v>
       </c>
       <c r="I25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="1">
         <v>43373</v>
       </c>
       <c r="B26">
         <v>65</v>
       </c>
       <c r="I26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B27">
+        <v>66</v>
+      </c>
+      <c r="I27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43374</v>
+      </c>
+      <c r="B28">
+        <v>67</v>
+      </c>
+      <c r="I28" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Audio reproduction notebook for complex nbr models
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E6A91BF-9E74-47EF-A380-97A01FD0FC12}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84F38B39-4321-438E-B381-322152BC5CEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -170,12 +170,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -199,6 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +523,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,22 +858,22 @@
       <c r="B15" s="3">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>5.8499455248008101E-3</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>-4.9414299214992896</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>-2.9187624359262498</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="4">
         <v>8.0849444575939504</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>-6.4876311729494796E-4</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -899,22 +906,22 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>3.9196163864368798E-3</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>0.10210658794458299</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>6.2019812058338104</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="4">
         <v>4.9962338577947696</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4">
         <v>5.0428877463265804</v>
       </c>
       <c r="I17" s="3"/>

</xml_diff>

<commit_message>
config for basic capsnet uniit test
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CEC608A3-8BC8-413A-9039-FC85E6A71676}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CA61882C-22DF-48D4-8F4C-BADA29FD7EE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Experiment</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Overtrain test on small complex capsunet with skips, continuation of 69</t>
   </si>
 </sst>
 </file>
@@ -523,10 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,18 +1154,163 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+      <c r="A29" s="3">
         <v>43374</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>69</v>
       </c>
-      <c r="I29" t="s">
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29">
+        <v>0.17299683392047799</v>
+      </c>
+      <c r="E29">
+        <v>5.1884083179774203</v>
+      </c>
+      <c r="F29">
+        <v>5.5859499771889798</v>
+      </c>
+      <c r="G29">
+        <v>18.750808889956499</v>
+      </c>
+      <c r="H29">
+        <v>-0.42715843088559702</v>
+      </c>
+      <c r="I29" s="4" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30">
+        <v>0.17299683392047799</v>
+      </c>
+      <c r="E30">
+        <v>12.606583273799499</v>
+      </c>
+      <c r="F30">
+        <v>14.2394586516382</v>
+      </c>
+      <c r="G30">
+        <v>18.890979882341799</v>
+      </c>
+      <c r="H30">
+        <v>-1.39254679747073</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4"/>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <v>0.124415507912635</v>
+      </c>
+      <c r="E31">
+        <v>5.6016612816488403</v>
+      </c>
+      <c r="F31">
+        <v>6.23286927430504</v>
+      </c>
+      <c r="G31">
+        <v>16.773685737918001</v>
+      </c>
+      <c r="H31">
+        <v>-1.3905467214172899E-2</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <v>0.124415507912635</v>
+      </c>
+      <c r="E32">
+        <v>13.5684510317638</v>
+      </c>
+      <c r="F32">
+        <v>14.5010678414389</v>
+      </c>
+      <c r="G32">
+        <v>21.780093642622202</v>
+      </c>
+      <c r="H32">
+        <v>-0.43067903950646202</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>43374</v>
+      </c>
+      <c r="B33" s="4">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>0.1219980224967</v>
+      </c>
+      <c r="E33">
+        <v>5.7841634420656298</v>
+      </c>
+      <c r="F33">
+        <v>6.9637912546762104</v>
+      </c>
+      <c r="G33">
+        <v>13.9138187244122</v>
+      </c>
+      <c r="H33">
+        <v>0.168596693202613</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>0.1219980224967</v>
+      </c>
+      <c r="E34">
+        <v>13.5938248385453</v>
+      </c>
+      <c r="F34">
+        <v>14.7032812981997</v>
+      </c>
+      <c r="G34">
+        <v>20.7402932165711</v>
+      </c>
+      <c r="H34">
+        <v>-0.405305232724961</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="21">
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>

</xml_diff>

<commit_message>
Added epsilon to squash
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{71F0E082-F9D9-48ED-BCEB-FAC8B12EDECC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C0CCB7E2-8B97-460D-8DA0-018666077A58}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="78">
   <si>
     <t>Experiment</t>
   </si>
@@ -259,10 +259,7 @@
     <t>Complex Number Capsnet</t>
   </si>
   <si>
-    <t>Metrics running on Africa</t>
-  </si>
-  <si>
-    <t>Final test (after 9 epochs) metrics runing oAmerica</t>
+    <t>Running on Asia</t>
   </si>
 </sst>
 </file>
@@ -333,10 +330,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,8 +653,8 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +830,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -859,7 +856,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -880,10 +877,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>43367</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="7">
         <v>50</v>
       </c>
       <c r="C11">
@@ -909,8 +906,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -934,10 +931,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>43368</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="7">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -958,13 +955,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -983,13 +980,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>43369</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="7">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1010,13 +1007,13 @@
       <c r="H15" s="2">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1035,11 +1032,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1058,11 +1055,11 @@
       <c r="H17" s="2">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="6"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1081,13 +1078,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="6"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>43370</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="7">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -1108,13 +1105,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -1133,13 +1130,13 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>43373</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="7">
         <v>61</v>
       </c>
       <c r="C21" t="s">
@@ -1160,13 +1157,13 @@
       <c r="H21">
         <v>8.5946525098830606E-3</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -1185,11 +1182,11 @@
       <c r="H22">
         <v>3.6873848603017803E-2</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
@@ -1208,11 +1205,11 @@
       <c r="H23">
         <v>0.78472849400813605</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -1231,7 +1228,7 @@
       <c r="H24">
         <v>2.0282006372733901E-2</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -1281,10 +1278,10 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>43374</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="7">
         <v>69</v>
       </c>
       <c r="C29" t="s">
@@ -1305,13 +1302,13 @@
       <c r="H29">
         <v>-0.42715843088559702</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -1330,11 +1327,11 @@
       <c r="H30">
         <v>-1.39254679747073</v>
       </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
@@ -1353,11 +1350,11 @@
       <c r="H31">
         <v>-1.3905467214172899E-2</v>
       </c>
-      <c r="I31" s="6"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
       <c r="C32" t="s">
         <v>34</v>
       </c>
@@ -1376,13 +1373,13 @@
       <c r="H32">
         <v>-0.43067903950646202</v>
       </c>
-      <c r="I32" s="6"/>
+      <c r="I32" s="7"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>43374</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="7">
         <v>71</v>
       </c>
       <c r="C33" t="s">
@@ -1403,13 +1400,13 @@
       <c r="H33">
         <v>0.168596693202613</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -1428,13 +1425,13 @@
       <c r="H34">
         <v>-0.405305232724961</v>
       </c>
-      <c r="I34" s="6"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>43375</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="7">
         <v>72</v>
       </c>
       <c r="C35" t="s">
@@ -1455,13 +1452,13 @@
       <c r="H35">
         <v>2.8573537209870499E-2</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
       <c r="C36" t="s">
         <v>32</v>
       </c>
@@ -1480,11 +1477,11 @@
       <c r="H36">
         <v>-1.5467030651102999E-3</v>
       </c>
-      <c r="I36" s="6"/>
+      <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
       <c r="C37" t="s">
         <v>33</v>
       </c>
@@ -1503,11 +1500,11 @@
       <c r="H37" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="6"/>
+      <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
       <c r="C38" t="s">
         <v>34</v>
       </c>
@@ -1526,13 +1523,13 @@
       <c r="H38" t="s">
         <v>46</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>43375</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="7">
         <v>75</v>
       </c>
       <c r="C39" t="s">
@@ -1553,13 +1550,13 @@
       <c r="H39">
         <v>-4.8766321545198298E-3</v>
       </c>
-      <c r="I39" s="6" t="s">
+      <c r="I39" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
       <c r="C40" t="s">
         <v>32</v>
       </c>
@@ -1578,11 +1575,11 @@
       <c r="H40">
         <v>-3.3103179357002401E-3</v>
       </c>
-      <c r="I40" s="6"/>
+      <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -1601,11 +1598,11 @@
       <c r="H41">
         <v>0.101846056595177</v>
       </c>
-      <c r="I41" s="6"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1624,7 +1621,7 @@
       <c r="H42">
         <v>6.0922125915421697E-2</v>
       </c>
-      <c r="I42" s="6"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -1807,42 +1804,117 @@
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="A52" s="6">
         <v>43377</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="7">
         <v>85</v>
       </c>
       <c r="C52" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52">
+        <v>8.8769710273481905E-3</v>
+      </c>
+      <c r="E52">
+        <v>-4.4486933776710904</v>
+      </c>
+      <c r="F52">
+        <v>-2.6658631119058098</v>
+      </c>
+      <c r="G52">
+        <v>8.5482997649644705</v>
+      </c>
+      <c r="H52">
+        <v>-1.5016279769943E-2</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="6"/>
+      <c r="B53" s="7"/>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D53">
+        <v>8.8769710273481905E-3</v>
+      </c>
+      <c r="E53">
+        <v>1.15316280088379</v>
+      </c>
+      <c r="F53">
+        <v>5.3171892248921999</v>
+      </c>
+      <c r="G53">
+        <v>8.5446161713002304</v>
+      </c>
+      <c r="H53">
+        <v>2.0442723267735299E-2</v>
+      </c>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>43378</v>
+      </c>
+      <c r="B54" s="7">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54">
+        <v>6.0007950481425097E-3</v>
+      </c>
+      <c r="E54">
+        <v>0.53187985334754795</v>
+      </c>
+      <c r="F54">
+        <v>6.2616599956293602</v>
+      </c>
+      <c r="G54">
+        <v>5.3511069949812704</v>
+      </c>
+      <c r="H54">
+        <v>4.9655569512486801</v>
+      </c>
+      <c r="I54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55">
+        <v>6.0007950481425097E-3</v>
+      </c>
+      <c r="E55">
+        <v>4.78322596010337</v>
+      </c>
+      <c r="F55">
+        <v>13.387147861798701</v>
+      </c>
+      <c r="G55">
+        <v>6.5279267189934798</v>
+      </c>
+      <c r="H55">
+        <v>3.6505058824873098</v>
+      </c>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43378</v>
+      </c>
+      <c r="B56">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
         <v>77</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="6"/>
-      <c r="I53" s="6"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
-        <v>43378</v>
-      </c>
-      <c r="B54" s="6">
-        <v>86</v>
-      </c>
-      <c r="C54" t="s">
-        <v>78</v>
-      </c>
-      <c r="I54" s="6"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="6"/>
-      <c r="I55" s="6"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I56" t="s">
         <v>74</v>
       </c>
@@ -1859,12 +1931,17 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="I39:I42"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>
@@ -1880,17 +1957,12 @@
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged caps unet changes
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E2467691-E870-4655-9A5D-0714732E69A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{571FA047-12A1-4BB0-AB29-E7815CCA4A6C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="87">
   <si>
     <t>Experiment</t>
   </si>
@@ -247,9 +247,6 @@
     <t>Unet</t>
   </si>
   <si>
-    <t>Patch Window: 128, Patch Hop: 64, Learning Rate: 0.002, Data Set: CHiME and LibriSpeech M</t>
-  </si>
-  <si>
     <t>Basic Capsnet</t>
   </si>
   <si>
@@ -260,6 +257,36 @@
   </si>
   <si>
     <t>Running on Asia</t>
+  </si>
+  <si>
+    <t>both (small LS)</t>
+  </si>
+  <si>
+    <t>U-Net</t>
+  </si>
+  <si>
+    <t>Try loading checkpoint 6 and testing</t>
+  </si>
+  <si>
+    <t>Metrics Running on America</t>
+  </si>
+  <si>
+    <t>Running on Africa</t>
+  </si>
+  <si>
+    <t>Caps-U-Net</t>
+  </si>
+  <si>
+    <t>Complex Caps-U-Net</t>
+  </si>
+  <si>
+    <t>16 KHz Experiments:</t>
+  </si>
+  <si>
+    <t>Patch Window: 256, Patch Hop: 128, Learning Rate: 0.0002, Data Set: CHiME and LibriSpeech S</t>
+  </si>
+  <si>
+    <t>Patch Window: 128, Patch Hop: 64, Learning Rate: 0.0002, Data Set: CHiME and LibriSpeech M</t>
   </si>
 </sst>
 </file>
@@ -336,10 +363,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -656,20 +683,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E56" sqref="E56"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -698,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>36</v>
       </c>
@@ -724,7 +751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>37</v>
       </c>
@@ -750,7 +777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>37</v>
       </c>
@@ -773,7 +800,7 @@
         <v>4.5625503126689404</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>40</v>
       </c>
@@ -796,7 +823,7 @@
         <v>1.01601424866862E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>40</v>
       </c>
@@ -819,7 +846,7 @@
         <v>5.2170367078359199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>48</v>
       </c>
@@ -827,7 +854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>49</v>
       </c>
@@ -835,8 +862,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -861,8 +888,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -882,11 +909,11 @@
         <v>9.9428347412899996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>43367</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="9">
         <v>50</v>
       </c>
       <c r="C11">
@@ -911,9 +938,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -936,11 +963,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
         <v>43368</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="9">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -961,13 +988,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -986,13 +1013,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
         <v>43369</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="9">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1013,13 +1040,13 @@
       <c r="H15" s="2">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1038,11 +1065,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1061,11 +1088,11 @@
       <c r="H17" s="2">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1084,13 +1111,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>43370</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="9">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -1111,13 +1138,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -1136,13 +1163,13 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>43373</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="9">
         <v>61</v>
       </c>
       <c r="C21" t="s">
@@ -1163,13 +1190,13 @@
       <c r="H21">
         <v>8.5946525098830606E-3</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -1188,11 +1215,11 @@
       <c r="H22">
         <v>3.6873848603017803E-2</v>
       </c>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
@@ -1211,11 +1238,11 @@
       <c r="H23">
         <v>0.78472849400813605</v>
       </c>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -1234,9 +1261,9 @@
       <c r="H24">
         <v>2.0282006372733901E-2</v>
       </c>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43373</v>
       </c>
@@ -1250,7 +1277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43373</v>
       </c>
@@ -1261,7 +1288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43374</v>
       </c>
@@ -1272,7 +1299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43374</v>
       </c>
@@ -1283,11 +1310,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
         <v>43374</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="9">
         <v>69</v>
       </c>
       <c r="C29" t="s">
@@ -1308,13 +1335,13 @@
       <c r="H29">
         <v>-0.42715843088559702</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -1333,11 +1360,11 @@
       <c r="H30">
         <v>-1.39254679747073</v>
       </c>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
@@ -1356,11 +1383,11 @@
       <c r="H31">
         <v>-1.3905467214172899E-2</v>
       </c>
-      <c r="I31" s="8"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
       <c r="C32" t="s">
         <v>34</v>
       </c>
@@ -1379,13 +1406,13 @@
       <c r="H32">
         <v>-0.43067903950646202</v>
       </c>
-      <c r="I32" s="8"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="9">
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
         <v>43374</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="9">
         <v>71</v>
       </c>
       <c r="C33" t="s">
@@ -1406,13 +1433,13 @@
       <c r="H33">
         <v>0.168596693202613</v>
       </c>
-      <c r="I33" s="8" t="s">
+      <c r="I33" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -1431,13 +1458,13 @@
       <c r="H34">
         <v>-0.405305232724961</v>
       </c>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="9">
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
         <v>43375</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" s="9">
         <v>72</v>
       </c>
       <c r="C35" t="s">
@@ -1458,13 +1485,13 @@
       <c r="H35">
         <v>2.8573537209870499E-2</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="9"/>
       <c r="C36" t="s">
         <v>32</v>
       </c>
@@ -1483,11 +1510,11 @@
       <c r="H36">
         <v>-1.5467030651102999E-3</v>
       </c>
-      <c r="I36" s="8"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9"/>
       <c r="C37" t="s">
         <v>33</v>
       </c>
@@ -1506,11 +1533,11 @@
       <c r="H37" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="8"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9"/>
       <c r="C38" t="s">
         <v>34</v>
       </c>
@@ -1529,13 +1556,13 @@
       <c r="H38" t="s">
         <v>46</v>
       </c>
-      <c r="I38" s="8"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="9">
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
         <v>43375</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="9">
         <v>75</v>
       </c>
       <c r="C39" t="s">
@@ -1556,13 +1583,13 @@
       <c r="H39">
         <v>-4.8766321545198298E-3</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="I39" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
       <c r="C40" t="s">
         <v>32</v>
       </c>
@@ -1581,11 +1608,11 @@
       <c r="H40">
         <v>-3.3103179357002401E-3</v>
       </c>
-      <c r="I40" s="8"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="8"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -1604,11 +1631,11 @@
       <c r="H41">
         <v>0.101846056595177</v>
       </c>
-      <c r="I41" s="8"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="8"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="9"/>
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1627,9 +1654,9 @@
       <c r="H42">
         <v>6.0922125915421697E-2</v>
       </c>
-      <c r="I42" s="8"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43376</v>
       </c>
@@ -1646,7 +1673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43376</v>
       </c>
@@ -1663,7 +1690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43376</v>
       </c>
@@ -1680,7 +1707,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43377</v>
       </c>
@@ -1709,7 +1736,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" t="s">
         <v>32</v>
@@ -1730,7 +1757,7 @@
         <v>0.619751518533326</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43377</v>
       </c>
@@ -1744,7 +1771,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43377</v>
       </c>
@@ -1773,7 +1800,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" t="s">
         <v>32</v>
@@ -1794,13 +1821,13 @@
         <v>0.69790060387249997</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>71</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1809,11 +1836,11 @@
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="9">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
         <v>43377</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" s="9">
         <v>85</v>
       </c>
       <c r="C52" t="s">
@@ -1834,13 +1861,13 @@
       <c r="H52">
         <v>-1.5016279769943E-2</v>
       </c>
-      <c r="I52" s="8" t="s">
+      <c r="I52" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="8"/>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
       <c r="C53" t="s">
         <v>32</v>
       </c>
@@ -1859,13 +1886,13 @@
       <c r="H53">
         <v>2.0442723267735299E-2</v>
       </c>
-      <c r="I53" s="8"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="9">
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
         <v>43378</v>
       </c>
-      <c r="B54" s="8">
+      <c r="B54" s="9">
         <v>89</v>
       </c>
       <c r="C54" t="s">
@@ -1886,11 +1913,11 @@
       <c r="H54">
         <v>4.9655569512486801</v>
       </c>
-      <c r="I54" s="8"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
-      <c r="B55" s="8"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
       <c r="C55" t="s">
         <v>32</v>
       </c>
@@ -1909,9 +1936,9 @@
       <c r="H55">
         <v>3.6505058824873098</v>
       </c>
-      <c r="I55" s="8"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="9"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" t="s">
@@ -1934,7 +1961,7 @@
       </c>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" t="s">
@@ -1957,7 +1984,7 @@
       </c>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43378</v>
       </c>
@@ -1965,30 +1992,85 @@
         <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I59" t="s">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I60" t="s">
-        <v>76</v>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>136</v>
+      </c>
+      <c r="C63" t="s">
+        <v>80</v>
+      </c>
+      <c r="I63" t="s">
+        <v>78</v>
+      </c>
+      <c r="J63" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>135</v>
+      </c>
+      <c r="C67" t="s">
+        <v>81</v>
+      </c>
+      <c r="I67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I75" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="I39:I42"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>
@@ -2004,17 +2086,12 @@
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="I52:I55"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2026,26 +2103,26 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2059,7 +2136,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2067,87 +2144,93 @@
         <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="M4">
-        <v>14987</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" t="s">
-        <v>63</v>
-      </c>
-      <c r="N5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="M5">
+        <v>14987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Setup to test unet 136 chkpt 6
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D13A820A-4AFC-43AC-93EB-033F5C2F7FCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7ADE3EC2-3999-485C-88A1-7783535E3758}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>Experiment</t>
   </si>
@@ -286,16 +286,13 @@
     <t>89 re-tested with corrected background noise estimation</t>
   </si>
   <si>
-    <t>metrics running on Africa</t>
-  </si>
-  <si>
-    <t>init test</t>
-  </si>
-  <si>
     <t>running on America</t>
   </si>
   <si>
     <t>Try loading at checkpoint 3 and testing</t>
+  </si>
+  <si>
+    <t>Same Unet as 136, but after 6 epochs</t>
   </si>
 </sst>
 </file>
@@ -359,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -372,10 +369,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -692,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomLeft" activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +917,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="10">
         <v>43367</v>
       </c>
       <c r="B11" s="9">
@@ -948,7 +946,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="9"/>
       <c r="C12">
         <v>0</v>
@@ -973,7 +971,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="10">
         <v>43368</v>
       </c>
       <c r="B13" s="9">
@@ -1002,7 +1000,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="9"/>
       <c r="C14" t="s">
         <v>32</v>
@@ -1025,7 +1023,7 @@
       <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="10">
         <v>43369</v>
       </c>
       <c r="B15" s="9">
@@ -1054,7 +1052,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="9"/>
       <c r="C16" t="s">
         <v>32</v>
@@ -1077,7 +1075,7 @@
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="9"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
@@ -1100,7 +1098,7 @@
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="9"/>
       <c r="C18" t="s">
         <v>34</v>
@@ -1123,7 +1121,7 @@
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="10">
         <v>43370</v>
       </c>
       <c r="B19" s="9">
@@ -1152,7 +1150,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="9"/>
       <c r="C20" t="s">
         <v>32</v>
@@ -1175,7 +1173,7 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="10">
         <v>43373</v>
       </c>
       <c r="B21" s="9">
@@ -1204,7 +1202,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="9"/>
       <c r="C22" t="s">
         <v>32</v>
@@ -1227,7 +1225,7 @@
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="9"/>
       <c r="C23" t="s">
         <v>33</v>
@@ -1250,7 +1248,7 @@
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="9"/>
       <c r="C24" t="s">
         <v>34</v>
@@ -1320,7 +1318,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="10">
         <v>43374</v>
       </c>
       <c r="B29" s="9">
@@ -1349,7 +1347,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="9"/>
       <c r="C30" t="s">
         <v>32</v>
@@ -1372,7 +1370,7 @@
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="9"/>
       <c r="C31" t="s">
         <v>33</v>
@@ -1395,7 +1393,7 @@
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="9"/>
       <c r="C32" t="s">
         <v>34</v>
@@ -1418,7 +1416,7 @@
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="10">
         <v>43374</v>
       </c>
       <c r="B33" s="9">
@@ -1447,7 +1445,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="9"/>
       <c r="C34" t="s">
         <v>32</v>
@@ -1470,7 +1468,7 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="10">
         <v>43375</v>
       </c>
       <c r="B35" s="9">
@@ -1499,7 +1497,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="9"/>
       <c r="C36" t="s">
         <v>32</v>
@@ -1522,7 +1520,7 @@
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="9"/>
       <c r="C37" t="s">
         <v>33</v>
@@ -1545,7 +1543,7 @@
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="9"/>
       <c r="C38" t="s">
         <v>34</v>
@@ -1568,7 +1566,7 @@
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="10">
         <v>43375</v>
       </c>
       <c r="B39" s="9">
@@ -1597,7 +1595,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="9"/>
       <c r="C40" t="s">
         <v>32</v>
@@ -1620,7 +1618,7 @@
       <c r="I40" s="9"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="10"/>
       <c r="B41" s="9"/>
       <c r="C41" t="s">
         <v>33</v>
@@ -1643,7 +1641,7 @@
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="9"/>
       <c r="C42" t="s">
         <v>34</v>
@@ -1846,7 +1844,7 @@
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="8">
+      <c r="A52" s="10">
         <v>43377</v>
       </c>
       <c r="B52" s="9">
@@ -1875,7 +1873,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="9"/>
       <c r="C53" t="s">
         <v>32</v>
@@ -1898,7 +1896,7 @@
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="8">
+      <c r="A54" s="10">
         <v>43378</v>
       </c>
       <c r="B54" s="9">
@@ -1925,7 +1923,7 @@
       <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="9"/>
       <c r="C55" t="s">
         <v>32</v>
@@ -2093,7 +2091,7 @@
       <c r="D65">
         <v>3.9452004128462496E-3</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="8">
         <v>6.8946836540872303</v>
       </c>
       <c r="F65">
@@ -2127,63 +2125,213 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="B67">
+        <v>140</v>
+      </c>
+      <c r="C67" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67">
+        <v>3.91506130246833E-3</v>
+      </c>
+      <c r="E67" s="2">
+        <v>6.9091884490599398</v>
+      </c>
+      <c r="F67">
+        <v>9.5183395249079101</v>
+      </c>
+      <c r="G67">
+        <v>14.14550056685</v>
+      </c>
+      <c r="H67">
+        <v>4.7624871892681799</v>
+      </c>
+      <c r="I67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68">
+        <v>3.91506130246833E-3</v>
+      </c>
+      <c r="E68">
+        <v>1.5156259629658799</v>
+      </c>
+      <c r="F68">
+        <v>7.7227375070833499</v>
+      </c>
+      <c r="G68">
+        <v>4.63777798002506</v>
+      </c>
+      <c r="H68">
+        <v>-3.2974368923159001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>43390</v>
       </c>
-      <c r="B67">
+      <c r="B69">
         <v>134</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
+        <v>31</v>
+      </c>
+      <c r="D69">
+        <v>6.1902719878231503E-3</v>
+      </c>
+      <c r="E69">
+        <v>2.1366363962492398</v>
+      </c>
+      <c r="F69">
+        <v>2.15475478958848</v>
+      </c>
+      <c r="G69">
+        <v>30.491525676382999</v>
+      </c>
+      <c r="H69">
+        <v>-1.00648635425107E-2</v>
+      </c>
+      <c r="I69" t="s">
+        <v>73</v>
+      </c>
+      <c r="J69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70">
+        <v>6.1902719878231503E-3</v>
+      </c>
+      <c r="E70">
+        <v>4.8153807699369402</v>
+      </c>
+      <c r="F70">
+        <v>4.8209386598883404</v>
+      </c>
+      <c r="G70">
+        <v>36.512190404000201</v>
+      </c>
+      <c r="H70">
+        <v>2.3179146551025099E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71">
+        <v>5.1723873604367704E-3</v>
+      </c>
+      <c r="E71" s="2">
+        <v>4.3668071185333099</v>
+      </c>
+      <c r="F71">
+        <v>5.7712948882694199</v>
+      </c>
+      <c r="G71">
+        <v>13.878630232213199</v>
+      </c>
+      <c r="H71">
+        <v>2.2201058587415501</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72">
+        <v>5.1723873604367704E-3</v>
+      </c>
+      <c r="E72">
+        <v>0.83181097526765602</v>
+      </c>
+      <c r="F72">
+        <v>7.0721564523653297</v>
+      </c>
+      <c r="G72">
+        <v>3.3994355973939898</v>
+      </c>
+      <c r="H72">
+        <v>-3.9812518800141699</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43391</v>
+      </c>
+      <c r="B73">
+        <v>137</v>
+      </c>
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73">
+        <v>6.7695307046343996E-3</v>
+      </c>
+      <c r="E73">
+        <v>2.1414376880545198</v>
+      </c>
+      <c r="F73">
+        <v>2.1425460966383101</v>
+      </c>
+      <c r="G73">
+        <v>42.893709838980101</v>
+      </c>
+      <c r="H73">
+        <v>-5.2635717372245903E-3</v>
+      </c>
+      <c r="I73" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>32</v>
+      </c>
+      <c r="D74">
+        <v>6.7695307046343996E-3</v>
+      </c>
+      <c r="E74">
+        <v>1.7148799301920099</v>
+      </c>
+      <c r="F74">
+        <v>4.0025226926442903</v>
+      </c>
+      <c r="G74">
+        <v>8.1402489827803599</v>
+      </c>
+      <c r="H74">
+        <v>-3.0981829250898101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>138</v>
+      </c>
+      <c r="C75" t="s">
         <v>86</v>
       </c>
-      <c r="I67" t="s">
-        <v>73</v>
-      </c>
-      <c r="J67" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>43391</v>
-      </c>
-      <c r="B71">
-        <v>137</v>
-      </c>
-      <c r="C71" t="s">
-        <v>87</v>
-      </c>
-      <c r="I71" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B73">
-        <v>138</v>
-      </c>
-      <c r="C73" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I75" t="s">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
         <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="I52:I55"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>
@@ -2199,12 +2347,18 @@
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="I52:I55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2216,7 +2370,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added function for L1 loss for phase
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7E364553-35E1-4ECD-B506-10BF0184FF96}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ACA48E4-75C3-4A69-8669-89A3E2505DA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
   <si>
     <t>Experiment</t>
   </si>
@@ -202,9 +203,6 @@
     <t>Repeat of 80, validation each epoch</t>
   </si>
   <si>
-    <t>Training iteration (batch size 50)</t>
-  </si>
-  <si>
     <t>CHiME</t>
   </si>
   <si>
@@ -284,12 +282,43 @@
   </si>
   <si>
     <t>Same Unet as 136, but after 6 epochs</t>
+  </si>
+  <si>
+    <t>Post-training</t>
+  </si>
+  <si>
+    <t>Pre-training</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Test Time</t>
+  </si>
+  <si>
+    <t>Training iterations/epoch (batch size --&gt;)</t>
+  </si>
+  <si>
+    <t>Complex U-Net</t>
+  </si>
+  <si>
+    <t>R-I-M U-Net</t>
+  </si>
+  <si>
+    <t>R-I-M Caps-U-Net</t>
+  </si>
+  <si>
+    <t>Mag and Phase, ouput Phase Difference?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -335,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -343,11 +372,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -361,11 +525,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,20 +864,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -723,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>36</v>
       </c>
@@ -749,7 +932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>37</v>
       </c>
@@ -775,7 +958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>37</v>
       </c>
@@ -798,7 +981,7 @@
         <v>4.5625503126689404</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>40</v>
       </c>
@@ -821,7 +1004,7 @@
         <v>1.01601424866862E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>40</v>
       </c>
@@ -844,7 +1027,7 @@
         <v>5.2170367078359199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>48</v>
       </c>
@@ -852,7 +1035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>49</v>
       </c>
@@ -860,8 +1043,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -886,8 +1069,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="23"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -907,11 +1090,11 @@
         <v>9.9428347412899996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="22">
         <v>43367</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="23">
         <v>50</v>
       </c>
       <c r="C11">
@@ -936,9 +1119,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -961,11 +1144,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="22">
         <v>43368</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="23">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -986,13 +1169,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -1011,13 +1194,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="10"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="I14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
         <v>43369</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="23">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1038,13 +1221,13 @@
       <c r="H15" s="2">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1063,11 +1246,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="10"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1086,11 +1269,11 @@
       <c r="H17" s="2">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
+      <c r="I17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1109,13 +1292,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="22">
         <v>43370</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="23">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -1136,13 +1319,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -1161,13 +1344,13 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="22">
         <v>43373</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="23">
         <v>61</v>
       </c>
       <c r="C21" t="s">
@@ -1188,13 +1371,13 @@
       <c r="H21">
         <v>8.5946525098830606E-3</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="10"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -1213,11 +1396,11 @@
       <c r="H22">
         <v>3.6873848603017803E-2</v>
       </c>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="10"/>
+      <c r="I22" s="23"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
@@ -1236,11 +1419,11 @@
       <c r="H23">
         <v>0.78472849400813605</v>
       </c>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
+      <c r="I23" s="23"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="22"/>
+      <c r="B24" s="23"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -1259,9 +1442,9 @@
       <c r="H24">
         <v>2.0282006372733901E-2</v>
       </c>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="23"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43373</v>
       </c>
@@ -1275,7 +1458,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43373</v>
       </c>
@@ -1286,7 +1469,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43374</v>
       </c>
@@ -1297,7 +1480,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>43374</v>
       </c>
@@ -1308,11 +1491,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="22">
         <v>43374</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="23">
         <v>69</v>
       </c>
       <c r="C29" t="s">
@@ -1333,13 +1516,13 @@
       <c r="H29">
         <v>-0.42715843088559702</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="10"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -1358,11 +1541,11 @@
       <c r="H30">
         <v>-1.39254679747073</v>
       </c>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="10"/>
+      <c r="I30" s="23"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
@@ -1381,11 +1564,11 @@
       <c r="H31">
         <v>-1.3905467214172899E-2</v>
       </c>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
       <c r="C32" t="s">
         <v>34</v>
       </c>
@@ -1404,13 +1587,13 @@
       <c r="H32">
         <v>-0.43067903950646202</v>
       </c>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="22">
         <v>43374</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="23">
         <v>71</v>
       </c>
       <c r="C33" t="s">
@@ -1431,13 +1614,13 @@
       <c r="H33">
         <v>0.168596693202613</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I33" s="23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -1456,13 +1639,13 @@
       <c r="H34">
         <v>-0.405305232724961</v>
       </c>
-      <c r="I34" s="10"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="22">
         <v>43375</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="23">
         <v>72</v>
       </c>
       <c r="C35" t="s">
@@ -1483,13 +1666,13 @@
       <c r="H35">
         <v>2.8573537209870499E-2</v>
       </c>
-      <c r="I35" s="10" t="s">
+      <c r="I35" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="22"/>
+      <c r="B36" s="23"/>
       <c r="C36" t="s">
         <v>32</v>
       </c>
@@ -1508,11 +1691,11 @@
       <c r="H36">
         <v>-1.5467030651102999E-3</v>
       </c>
-      <c r="I36" s="10"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
+      <c r="I36" s="23"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
       <c r="C37" t="s">
         <v>33</v>
       </c>
@@ -1531,11 +1714,11 @@
       <c r="H37" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="10"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="10"/>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
       <c r="C38" t="s">
         <v>34</v>
       </c>
@@ -1554,13 +1737,13 @@
       <c r="H38" t="s">
         <v>46</v>
       </c>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="22">
         <v>43375</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="23">
         <v>75</v>
       </c>
       <c r="C39" t="s">
@@ -1581,13 +1764,13 @@
       <c r="H39">
         <v>-4.8766321545198298E-3</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="23" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="10"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="22"/>
+      <c r="B40" s="23"/>
       <c r="C40" t="s">
         <v>32</v>
       </c>
@@ -1606,11 +1789,11 @@
       <c r="H40">
         <v>-3.3103179357002401E-3</v>
       </c>
-      <c r="I40" s="10"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
-      <c r="B41" s="10"/>
+      <c r="I40" s="23"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="22"/>
+      <c r="B41" s="23"/>
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -1629,11 +1812,11 @@
       <c r="H41">
         <v>0.101846056595177</v>
       </c>
-      <c r="I41" s="10"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
-      <c r="B42" s="10"/>
+      <c r="I41" s="23"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="22"/>
+      <c r="B42" s="23"/>
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1652,9 +1835,9 @@
       <c r="H42">
         <v>6.0922125915421697E-2</v>
       </c>
-      <c r="I42" s="10"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43376</v>
       </c>
@@ -1671,7 +1854,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43376</v>
       </c>
@@ -1688,7 +1871,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43376</v>
       </c>
@@ -1705,7 +1888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>43377</v>
       </c>
@@ -1734,7 +1917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="C47" t="s">
         <v>32</v>
@@ -1755,7 +1938,7 @@
         <v>0.619751518533326</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>43377</v>
       </c>
@@ -1769,7 +1952,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>43377</v>
       </c>
@@ -1795,10 +1978,10 @@
         <v>1.69316821399544</v>
       </c>
       <c r="I49" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="C50" t="s">
         <v>32</v>
@@ -1819,7 +2002,7 @@
         <v>0.69790060387249997</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51">
         <v>145</v>
@@ -1843,7 +2026,7 @@
         <v>-0.31863876639355398</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="C52" t="s">
         <v>32</v>
@@ -1864,7 +2047,7 @@
         <v>2.67662389686584</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="C53" t="s">
         <v>33</v>
@@ -1885,7 +2068,7 @@
         <v>0.95464630209159695</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="C54" t="s">
         <v>34</v>
@@ -1906,7 +2089,7 @@
         <v>4.8512619602994098</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55">
         <v>146</v>
@@ -1930,7 +2113,7 @@
         <v>-0.56767955034740303</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="C56" t="s">
         <v>32</v>
@@ -1951,7 +2134,7 @@
         <v>1.8761231724104801</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="C57" t="s">
         <v>33</v>
@@ -1972,7 +2155,7 @@
         <v>0.76717154068581295</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="C58" t="s">
         <v>34</v>
@@ -1993,13 +2176,13 @@
         <v>3.8964804606254</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -2008,11 +2191,11 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="22">
         <v>43377</v>
       </c>
-      <c r="B60" s="10">
+      <c r="B60" s="23">
         <v>85</v>
       </c>
       <c r="C60" t="s">
@@ -2033,13 +2216,13 @@
       <c r="H60">
         <v>-1.5016279769943E-2</v>
       </c>
-      <c r="I60" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
-      <c r="B61" s="10"/>
+      <c r="I60" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="22"/>
+      <c r="B61" s="23"/>
       <c r="C61" t="s">
         <v>32</v>
       </c>
@@ -2058,13 +2241,13 @@
       <c r="H61">
         <v>2.0442723267735299E-2</v>
       </c>
-      <c r="I61" s="10"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="9">
+      <c r="I61" s="23"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="22">
         <v>43378</v>
       </c>
-      <c r="B62" s="10">
+      <c r="B62" s="23">
         <v>89</v>
       </c>
       <c r="C62" t="s">
@@ -2085,11 +2268,11 @@
       <c r="H62">
         <v>4.9655569512486801</v>
       </c>
-      <c r="I62" s="10"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
+      <c r="I62" s="23"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="22"/>
+      <c r="B63" s="23"/>
       <c r="C63" t="s">
         <v>32</v>
       </c>
@@ -2108,9 +2291,9 @@
       <c r="H63">
         <v>3.6505058824873098</v>
       </c>
-      <c r="I63" s="10"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" t="s">
@@ -2131,11 +2314,11 @@
       <c r="H64">
         <v>4.5462062693628003</v>
       </c>
-      <c r="I64" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I64" s="23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" t="s">
@@ -2156,15 +2339,15 @@
       <c r="H65">
         <v>-3.4906857233533901</v>
       </c>
-      <c r="I65" s="10"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I65" s="23"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2173,7 +2356,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>43388</v>
       </c>
@@ -2199,13 +2382,13 @@
         <v>-6.32791094461188E-3</v>
       </c>
       <c r="I68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>32</v>
       </c>
@@ -2225,7 +2408,7 @@
         <v>-3.28339441892745</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
         <v>33</v>
       </c>
@@ -2245,7 +2428,7 @@
         <v>4.7479823942955202</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
         <v>34</v>
       </c>
@@ -2265,7 +2448,7 @@
         <v>-3.20942124047644</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>140</v>
       </c>
@@ -2288,10 +2471,10 @@
         <v>4.7624871892681799</v>
       </c>
       <c r="I72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>32</v>
       </c>
@@ -2311,7 +2494,7 @@
         <v>-3.2974368923159001</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>43390</v>
       </c>
@@ -2337,13 +2520,13 @@
         <v>-1.00648635425107E-2</v>
       </c>
       <c r="I74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J74" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
         <v>32</v>
       </c>
@@ -2363,7 +2546,7 @@
         <v>2.3179146551025099E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>33</v>
       </c>
@@ -2383,7 +2566,7 @@
         <v>2.2201058587415501</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
         <v>34</v>
       </c>
@@ -2403,7 +2586,7 @@
         <v>-3.9812518800141699</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>43391</v>
       </c>
@@ -2429,10 +2612,10 @@
         <v>-5.2635717372245903E-3</v>
       </c>
       <c r="I78" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
         <v>32</v>
       </c>
@@ -2452,17 +2635,40 @@
         <v>-3.0981829250898101</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>138</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>82</v>
+      </c>
       <c r="I82" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I83" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="I86" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2507,30 +2713,180 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF23902-3816-4B4E-83CE-581E9B6C3F52}">
+  <dimension ref="B1:H6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="10">
+        <v>5.8508186126840396E-3</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2.1403733488471399</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2.14143031615124</v>
+      </c>
+      <c r="G3" s="11">
+        <v>43.1675045082523</v>
+      </c>
+      <c r="H3" s="16">
+        <v>-6.32791094461188E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="24"/>
+      <c r="C4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="10">
+        <v>3.91506130246833E-3</v>
+      </c>
+      <c r="E4" s="12">
+        <v>6.9091884490599398</v>
+      </c>
+      <c r="F4" s="11">
+        <v>9.5183395249079101</v>
+      </c>
+      <c r="G4" s="11">
+        <v>14.14550056685</v>
+      </c>
+      <c r="H4" s="16">
+        <v>4.7624871892681799</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6.1902719878231503E-3</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.1366363962492398</v>
+      </c>
+      <c r="F5" s="11">
+        <v>2.15475478958848</v>
+      </c>
+      <c r="G5" s="11">
+        <v>30.491525676382999</v>
+      </c>
+      <c r="H5" s="16">
+        <v>-1.00648635425107E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="25"/>
+      <c r="C6" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="18">
+        <v>5.1723873604367704E-3</v>
+      </c>
+      <c r="E6" s="19">
+        <v>4.3668071185333099</v>
+      </c>
+      <c r="F6" s="20">
+        <v>5.7712948882694199</v>
+      </c>
+      <c r="G6" s="20">
+        <v>13.878630232213199</v>
+      </c>
+      <c r="H6" s="21">
+        <v>2.2201058587415501</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB077578-BE78-4B93-9E5A-D84D4BCC6A7F}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L2" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2538,13 +2894,13 @@
         <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M3">
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2552,93 +2908,99 @@
         <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M4">
         <v>4800</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>80000</v>
+      </c>
+      <c r="O4">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M5">
         <v>14987</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" t="s">
         <v>63</v>
       </c>
-      <c r="N6" t="s">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Trying to fix inputs
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8ACA48E4-75C3-4A69-8669-89A3E2505DA6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9A20CA5E-0535-46EC-8CA1-0142F0411B85}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t>Experiment</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>Mag and Phase, ouput Phase Difference?</t>
+  </si>
+  <si>
+    <t>Overtraining efforts with complex capsunet</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -867,17 +870,17 @@
   <dimension ref="A1:J86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="81.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -906,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>36</v>
       </c>
@@ -932,7 +935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>37</v>
       </c>
@@ -958,7 +961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>37</v>
       </c>
@@ -981,7 +984,7 @@
         <v>4.5625503126689404</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>40</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>1.01601424866862E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>40</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>5.2170367078359199</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>48</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>49</v>
       </c>
@@ -1043,8 +1046,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C9">
@@ -1069,8 +1072,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
       <c r="C10">
         <v>1</v>
       </c>
@@ -1090,11 +1093,11 @@
         <v>9.9428347412899996</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
         <v>43367</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>50</v>
       </c>
       <c r="C11">
@@ -1119,9 +1122,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12">
         <v>0</v>
       </c>
@@ -1144,11 +1147,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
         <v>43368</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>51</v>
       </c>
       <c r="C13" t="s">
@@ -1169,13 +1172,13 @@
       <c r="H13">
         <v>5.1734518444775501</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="22"/>
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -1194,13 +1197,13 @@
       <c r="H14">
         <v>3.7281922612481901</v>
       </c>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
         <v>43369</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1221,13 +1224,13 @@
       <c r="H15" s="2">
         <v>-6.4876311729494796E-4</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22"/>
       <c r="C16" t="s">
         <v>32</v>
       </c>
@@ -1246,11 +1249,11 @@
       <c r="H16">
         <v>1.54551858325779E-2</v>
       </c>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
+      <c r="I16" s="22"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1269,11 +1272,11 @@
       <c r="H17" s="2">
         <v>5.0428877463265804</v>
       </c>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="22"/>
       <c r="C18" t="s">
         <v>34</v>
       </c>
@@ -1292,13 +1295,13 @@
       <c r="H18">
         <v>3.58423085463872</v>
       </c>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="22">
+      <c r="I18" s="22"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
         <v>43370</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <v>54</v>
       </c>
       <c r="C19" t="s">
@@ -1319,13 +1322,13 @@
       <c r="H19">
         <v>2.3427632342802398</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="I19" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="22"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
@@ -1344,13 +1347,13 @@
       <c r="H20">
         <v>0.194433594332584</v>
       </c>
-      <c r="I20" s="23"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="22">
+      <c r="I20" s="22"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="23">
         <v>43373</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>61</v>
       </c>
       <c r="C21" t="s">
@@ -1371,13 +1374,13 @@
       <c r="H21">
         <v>8.5946525098830606E-3</v>
       </c>
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="23"/>
+      <c r="B22" s="22"/>
       <c r="C22" t="s">
         <v>32</v>
       </c>
@@ -1396,11 +1399,11 @@
       <c r="H22">
         <v>3.6873848603017803E-2</v>
       </c>
-      <c r="I22" s="23"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
+      <c r="I22" s="22"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="22"/>
       <c r="C23" t="s">
         <v>33</v>
       </c>
@@ -1419,11 +1422,11 @@
       <c r="H23">
         <v>0.78472849400813605</v>
       </c>
-      <c r="I23" s="23"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
+      <c r="I23" s="22"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="22"/>
       <c r="C24" t="s">
         <v>34</v>
       </c>
@@ -1442,9 +1445,9 @@
       <c r="H24">
         <v>2.0282006372733901E-2</v>
       </c>
-      <c r="I24" s="23"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I24" s="22"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43373</v>
       </c>
@@ -1458,7 +1461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43373</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43374</v>
       </c>
@@ -1480,7 +1483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43374</v>
       </c>
@@ -1491,11 +1494,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="23">
         <v>43374</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>69</v>
       </c>
       <c r="C29" t="s">
@@ -1516,13 +1519,13 @@
       <c r="H29">
         <v>-0.42715843088559702</v>
       </c>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="22"/>
       <c r="C30" t="s">
         <v>32</v>
       </c>
@@ -1541,11 +1544,11 @@
       <c r="H30">
         <v>-1.39254679747073</v>
       </c>
-      <c r="I30" s="23"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
+      <c r="I30" s="22"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="22"/>
       <c r="C31" t="s">
         <v>33</v>
       </c>
@@ -1564,11 +1567,11 @@
       <c r="H31">
         <v>-1.3905467214172899E-2</v>
       </c>
-      <c r="I31" s="23"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
+      <c r="I31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="22"/>
       <c r="C32" t="s">
         <v>34</v>
       </c>
@@ -1587,13 +1590,13 @@
       <c r="H32">
         <v>-0.43067903950646202</v>
       </c>
-      <c r="I32" s="23"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="22">
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
         <v>43374</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="22">
         <v>71</v>
       </c>
       <c r="C33" t="s">
@@ -1614,13 +1617,13 @@
       <c r="H33">
         <v>0.168596693202613</v>
       </c>
-      <c r="I33" s="23" t="s">
+      <c r="I33" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="22"/>
       <c r="C34" t="s">
         <v>32</v>
       </c>
@@ -1639,13 +1642,13 @@
       <c r="H34">
         <v>-0.405305232724961</v>
       </c>
-      <c r="I34" s="23"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="22">
+      <c r="I34" s="22"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
         <v>43375</v>
       </c>
-      <c r="B35" s="23">
+      <c r="B35" s="22">
         <v>72</v>
       </c>
       <c r="C35" t="s">
@@ -1666,13 +1669,13 @@
       <c r="H35">
         <v>2.8573537209870499E-2</v>
       </c>
-      <c r="I35" s="23" t="s">
+      <c r="I35" s="22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
-      <c r="B36" s="23"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="22"/>
       <c r="C36" t="s">
         <v>32</v>
       </c>
@@ -1691,11 +1694,11 @@
       <c r="H36">
         <v>-1.5467030651102999E-3</v>
       </c>
-      <c r="I36" s="23"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
+      <c r="I36" s="22"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="22"/>
       <c r="C37" t="s">
         <v>33</v>
       </c>
@@ -1714,11 +1717,11 @@
       <c r="H37" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="23"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="22"/>
       <c r="C38" t="s">
         <v>34</v>
       </c>
@@ -1737,13 +1740,13 @@
       <c r="H38" t="s">
         <v>46</v>
       </c>
-      <c r="I38" s="23"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="22">
+      <c r="I38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="23">
         <v>43375</v>
       </c>
-      <c r="B39" s="23">
+      <c r="B39" s="22">
         <v>75</v>
       </c>
       <c r="C39" t="s">
@@ -1764,13 +1767,13 @@
       <c r="H39">
         <v>-4.8766321545198298E-3</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="22"/>
       <c r="C40" t="s">
         <v>32</v>
       </c>
@@ -1789,11 +1792,11 @@
       <c r="H40">
         <v>-3.3103179357002401E-3</v>
       </c>
-      <c r="I40" s="23"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="23"/>
+      <c r="I40" s="22"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="22"/>
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -1812,11 +1815,11 @@
       <c r="H41">
         <v>0.101846056595177</v>
       </c>
-      <c r="I41" s="23"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
+      <c r="I41" s="22"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="22"/>
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1835,9 +1838,9 @@
       <c r="H42">
         <v>6.0922125915421697E-2</v>
       </c>
-      <c r="I42" s="23"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="22"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43376</v>
       </c>
@@ -1854,7 +1857,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43376</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43376</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43377</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" t="s">
         <v>32</v>
@@ -1938,7 +1941,7 @@
         <v>0.619751518533326</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43377</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43377</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" t="s">
         <v>32</v>
@@ -2002,7 +2005,7 @@
         <v>0.69790060387249997</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51">
         <v>145</v>
@@ -2025,8 +2028,11 @@
       <c r="H51">
         <v>-0.31863876639355398</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="C52" t="s">
         <v>32</v>
@@ -2046,8 +2052,9 @@
       <c r="H52">
         <v>2.67662389686584</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I52" s="22"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="C53" t="s">
         <v>33</v>
@@ -2067,8 +2074,9 @@
       <c r="H53">
         <v>0.95464630209159695</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I53" s="22"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" t="s">
         <v>34</v>
@@ -2088,8 +2096,9 @@
       <c r="H54">
         <v>4.8512619602994098</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I54" s="22"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55">
         <v>146</v>
@@ -2112,8 +2121,9 @@
       <c r="H55">
         <v>-0.56767955034740303</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I55" s="22"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="C56" t="s">
         <v>32</v>
@@ -2133,8 +2143,9 @@
       <c r="H56">
         <v>1.8761231724104801</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I56" s="22"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="C57" t="s">
         <v>33</v>
@@ -2154,8 +2165,9 @@
       <c r="H57">
         <v>0.76717154068581295</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I57" s="22"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="C58" t="s">
         <v>34</v>
@@ -2175,8 +2187,9 @@
       <c r="H58">
         <v>3.8964804606254</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I58" s="22"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>70</v>
       </c>
@@ -2191,11 +2204,11 @@
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="22">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="23">
         <v>43377</v>
       </c>
-      <c r="B60" s="23">
+      <c r="B60" s="22">
         <v>85</v>
       </c>
       <c r="C60" t="s">
@@ -2216,13 +2229,13 @@
       <c r="H60">
         <v>-1.5016279769943E-2</v>
       </c>
-      <c r="I60" s="23" t="s">
+      <c r="I60" s="22" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
-      <c r="B61" s="23"/>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="B61" s="22"/>
       <c r="C61" t="s">
         <v>32</v>
       </c>
@@ -2241,13 +2254,13 @@
       <c r="H61">
         <v>2.0442723267735299E-2</v>
       </c>
-      <c r="I61" s="23"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="22">
+      <c r="I61" s="22"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="23">
         <v>43378</v>
       </c>
-      <c r="B62" s="23">
+      <c r="B62" s="22">
         <v>89</v>
       </c>
       <c r="C62" t="s">
@@ -2268,11 +2281,11 @@
       <c r="H62">
         <v>4.9655569512486801</v>
       </c>
-      <c r="I62" s="23"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
-      <c r="B63" s="23"/>
+      <c r="I62" s="22"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="B63" s="22"/>
       <c r="C63" t="s">
         <v>32</v>
       </c>
@@ -2291,9 +2304,9 @@
       <c r="H63">
         <v>3.6505058824873098</v>
       </c>
-      <c r="I63" s="23"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I63" s="22"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" t="s">
@@ -2314,11 +2327,11 @@
       <c r="H64">
         <v>4.5462062693628003</v>
       </c>
-      <c r="I64" s="23" t="s">
+      <c r="I64" s="22" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" t="s">
@@ -2339,9 +2352,9 @@
       <c r="H65">
         <v>-3.4906857233533901</v>
       </c>
-      <c r="I65" s="23"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I65" s="22"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>77</v>
       </c>
@@ -2356,7 +2369,7 @@
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43388</v>
       </c>
@@ -2388,7 +2401,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>32</v>
       </c>
@@ -2408,7 +2421,7 @@
         <v>-3.28339441892745</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>33</v>
       </c>
@@ -2428,7 +2441,7 @@
         <v>4.7479823942955202</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>34</v>
       </c>
@@ -2448,7 +2461,7 @@
         <v>-3.20942124047644</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>140</v>
       </c>
@@ -2474,7 +2487,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>32</v>
       </c>
@@ -2494,7 +2507,7 @@
         <v>-3.2974368923159001</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43390</v>
       </c>
@@ -2526,7 +2539,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>32</v>
       </c>
@@ -2546,7 +2559,7 @@
         <v>2.3179146551025099E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
         <v>33</v>
       </c>
@@ -2566,7 +2579,7 @@
         <v>2.2201058587415501</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
         <v>34</v>
       </c>
@@ -2586,7 +2599,7 @@
         <v>-3.9812518800141699</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43391</v>
       </c>
@@ -2615,7 +2628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
         <v>32</v>
       </c>
@@ -2635,7 +2648,7 @@
         <v>-3.0981829250898101</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>138</v>
       </c>
@@ -2643,7 +2656,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>82</v>
       </c>
@@ -2651,40 +2664,35 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I83" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I85" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
       <c r="I86" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="I60:I63"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="I39:I42"/>
+  <mergeCells count="34">
+    <mergeCell ref="I51:I58"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>
@@ -2700,12 +2708,18 @@
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="I60:I63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2720,19 +2734,19 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>87</v>
       </c>
@@ -2755,7 +2769,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>74</v>
       </c>
@@ -2778,7 +2792,7 @@
         <v>-6.32791094461188E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
       <c r="C4" s="9" t="s">
         <v>85</v>
@@ -2799,7 +2813,7 @@
         <v>4.7624871892681799</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>72</v>
       </c>
@@ -2822,7 +2836,7 @@
         <v>-1.00648635425107E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25"/>
       <c r="C6" s="17" t="s">
         <v>85</v>
@@ -2861,18 +2875,18 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L2" s="3" t="s">
         <v>89</v>
       </c>
@@ -2886,7 +2900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2900,7 +2914,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2934,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2931,7 +2945,7 @@
         <v>14987</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2945,62 +2959,62 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Results update from 149
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{51EC5CB1-7030-498F-8D87-9AC31E896986}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{630DCD0C-0EB8-4674-909D-0591D557B7B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" activeTab="2" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="95">
   <si>
     <t>Experiment</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>3 layer conv net</t>
-  </si>
-  <si>
-    <t>Metrics running on Eurpe</t>
   </si>
 </sst>
 </file>
@@ -870,11 +867,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FE2BEB-AFEC-4FDB-87E2-6A5999A2F15B}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2535,7 +2532,7 @@
       <c r="H74">
         <v>-1.00648635425107E-2</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I74" s="22" t="s">
         <v>72</v>
       </c>
       <c r="J74" t="s">
@@ -2561,6 +2558,7 @@
       <c r="H75">
         <v>2.3179146551025099E-3</v>
       </c>
+      <c r="I75" s="22"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
@@ -2581,6 +2579,7 @@
       <c r="H76">
         <v>2.2201058587415501</v>
       </c>
+      <c r="I76" s="22"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
@@ -2601,6 +2600,7 @@
       <c r="H77">
         <v>-3.9812518800141699</v>
       </c>
+      <c r="I77" s="22"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
@@ -2627,7 +2627,7 @@
       <c r="H78">
         <v>-5.2635717372245903E-3</v>
       </c>
-      <c r="I78" t="s">
+      <c r="I78" s="22" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2650,140 +2650,226 @@
       <c r="H79">
         <v>-3.0981829250898101</v>
       </c>
+      <c r="I79" s="22"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80">
         <v>149</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="D80">
-        <v>5.4999999999999997E-3</v>
-      </c>
+        <v>6.7223707032820802E-3</v>
+      </c>
+      <c r="E80">
+        <v>2.1405847224893</v>
+      </c>
+      <c r="F80">
+        <v>2.1416455561305701</v>
+      </c>
+      <c r="G80">
+        <v>43.136957872328097</v>
+      </c>
+      <c r="H80">
+        <v>-6.1165373024574896E-3</v>
+      </c>
+      <c r="I80" s="22"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>32</v>
+      </c>
+      <c r="D81">
+        <v>6.7223707032820802E-3</v>
+      </c>
+      <c r="E81">
+        <v>1.4768872015169801</v>
+      </c>
+      <c r="F81">
+        <v>3.7342455804076899</v>
+      </c>
+      <c r="G81">
+        <v>8.0191130714056698</v>
+      </c>
+      <c r="H81">
+        <v>-3.3361756537648399</v>
+      </c>
+      <c r="I81" s="22"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
-        <v>43398</v>
-      </c>
-      <c r="B82">
-        <v>154</v>
-      </c>
       <c r="C82" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D82">
-        <v>6.05322966534186E-3</v>
-      </c>
-      <c r="E82">
-        <v>1.88817622693805</v>
+        <v>5.5386539191398599E-3</v>
+      </c>
+      <c r="E82" s="2">
+        <v>4.2151008389608497</v>
       </c>
       <c r="F82">
-        <v>4.5345716021200797</v>
+        <v>4.4419299518815496</v>
       </c>
       <c r="G82">
-        <v>9.4648998759248695</v>
+        <v>20.275467288436801</v>
       </c>
       <c r="H82">
-        <v>-0.25852503285369899</v>
-      </c>
-      <c r="I82" t="s">
-        <v>94</v>
-      </c>
+        <v>2.0683995791691099</v>
+      </c>
+      <c r="I82" s="22"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D83">
+        <v>5.5386539191398599E-3</v>
+      </c>
+      <c r="E83">
+        <v>1.4451225758309401</v>
+      </c>
+      <c r="F83">
+        <v>6.9646341282037199</v>
+      </c>
+      <c r="G83">
+        <v>4.6972574976468602</v>
+      </c>
+      <c r="H83">
+        <v>-3.3679402794508602</v>
+      </c>
+      <c r="I83" s="22"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>43398</v>
+      </c>
+      <c r="B84">
+        <v>154</v>
+      </c>
+      <c r="C84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D84">
         <v>6.05322966534186E-3</v>
       </c>
-      <c r="E83">
-        <v>2.2926471838902902</v>
-      </c>
-      <c r="F83">
-        <v>5.8273145314643999</v>
-      </c>
-      <c r="G83">
-        <v>6.7401128385186402</v>
-      </c>
-      <c r="H83">
-        <v>-2.52041567139152</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C84" t="s">
-        <v>33</v>
-      </c>
-      <c r="D84">
-        <v>5.3014564192564702E-3</v>
-      </c>
       <c r="E84">
-        <v>1.8812702780464301</v>
+        <v>1.88817622693805</v>
       </c>
       <c r="F84">
-        <v>3.37891165486923</v>
+        <v>4.5345716021200797</v>
       </c>
       <c r="G84">
-        <v>10.942205468918701</v>
+        <v>9.4648998759248695</v>
       </c>
       <c r="H84">
-        <v>-0.26543098174531699</v>
+        <v>-0.25852503285369899</v>
+      </c>
+      <c r="I84" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
+        <v>32</v>
+      </c>
+      <c r="D85">
+        <v>6.05322966534186E-3</v>
+      </c>
+      <c r="E85">
+        <v>2.2926471838902902</v>
+      </c>
+      <c r="F85">
+        <v>5.8273145314643999</v>
+      </c>
+      <c r="G85">
+        <v>6.7401128385186402</v>
+      </c>
+      <c r="H85">
+        <v>-2.52041567139152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86">
+        <v>5.3014564192564702E-3</v>
+      </c>
+      <c r="E86">
+        <v>1.8812702780464301</v>
+      </c>
+      <c r="F86">
+        <v>3.37891165486923</v>
+      </c>
+      <c r="G86">
+        <v>10.942205468918701</v>
+      </c>
+      <c r="H86">
+        <v>-0.26543098174531699</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
         <v>34</v>
       </c>
-      <c r="D85">
+      <c r="D87">
         <v>5.3014564192564702E-3</v>
       </c>
-      <c r="E85">
+      <c r="E87">
         <v>3.3040239747320999</v>
       </c>
-      <c r="F85">
+      <c r="F87">
         <v>6.77711490653006</v>
       </c>
-      <c r="G85">
+      <c r="G87">
         <v>7.6874198379358001</v>
       </c>
-      <c r="H85">
+      <c r="H87">
         <v>-1.5090388805497199</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I86" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I87" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I88" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I91" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I92" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="I60:I63"/>
+  <mergeCells count="36">
+    <mergeCell ref="I78:I83"/>
+    <mergeCell ref="I74:I77"/>
+    <mergeCell ref="I51:I58"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="I39:I42"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="I21:I24"/>
@@ -2799,19 +2885,12 @@
     <mergeCell ref="I15:I18"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="I51:I58"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="I60:I63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -2963,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB077578-BE78-4B93-9E5A-D84D4BCC6A7F}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
phase_weight change and mag_phase_diff bug fix
</commit_message>
<xml_diff>
--- a/test_metrics/Results.xlsx
+++ b/test_metrics/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toby\MSc_Project\MScFinalProject\test_metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{70BD4429-BAB8-4AD6-8BDD-13548539E15A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{813617D7-BD88-40E4-80A7-5B2913E2E573}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="3990" windowHeight="4260" xr2:uid="{C09168AC-4653-4BBE-87AE-0F1A556ACEDC}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="173">
   <si>
     <t>Experiment</t>
   </si>
@@ -543,7 +543,10 @@
     <t>Queued on Europe</t>
   </si>
   <si>
-    <t>Metrics running on Africa</t>
+    <t>Re-run</t>
+  </si>
+  <si>
+    <t>Re-run?</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +622,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1140,6 +1149,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1656,7 +1667,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D184" sqref="D184"/>
+      <selection pane="bottomLeft" activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -4088,7 +4099,7 @@
       <c r="D122" s="64">
         <v>2.5172597916725101E-3</v>
       </c>
-      <c r="E122" s="64">
+      <c r="E122" s="78">
         <v>11.812966277372</v>
       </c>
       <c r="F122" s="64">
@@ -4143,7 +4154,7 @@
       <c r="D124" s="67">
         <v>2.4841721818889802E-3</v>
       </c>
-      <c r="E124" s="67">
+      <c r="E124" s="79">
         <v>11.903875779176801</v>
       </c>
       <c r="F124" s="67">
@@ -5276,8 +5287,23 @@
       <c r="B176">
         <v>218</v>
       </c>
-      <c r="C176" s="40">
-        <v>1.2700000000000001E-3</v>
+      <c r="C176" t="s">
+        <v>31</v>
+      </c>
+      <c r="D176">
+        <v>1.25862060208769E-3</v>
+      </c>
+      <c r="E176">
+        <v>11.825863725648</v>
+      </c>
+      <c r="F176">
+        <v>17.049876124890702</v>
+      </c>
+      <c r="G176">
+        <v>13.7065544208929</v>
+      </c>
+      <c r="H176">
+        <v>8.1497756189980404</v>
       </c>
       <c r="I176" s="64" t="s">
         <v>163</v>
@@ -5287,19 +5313,46 @@
       <c r="B177">
         <v>223</v>
       </c>
-      <c r="C177">
-        <v>1.258E-3</v>
-      </c>
-      <c r="D177" t="s">
-        <v>171</v>
+      <c r="C177" t="s">
+        <v>32</v>
+      </c>
+      <c r="D177">
+        <v>1.25862060208769E-3</v>
+      </c>
+      <c r="E177">
+        <v>3.53402527798352</v>
+      </c>
+      <c r="F177">
+        <v>6.9899142067291598</v>
+      </c>
+      <c r="G177">
+        <v>8.8541252810865707</v>
+      </c>
+      <c r="H177">
+        <v>6.4557605343573599</v>
       </c>
     </row>
     <row r="178" spans="2:9">
       <c r="B178">
         <v>220</v>
       </c>
-      <c r="C178" s="40">
-        <v>1.276E-3</v>
+      <c r="C178" t="s">
+        <v>31</v>
+      </c>
+      <c r="D178">
+        <v>1.2465816300111601E-3</v>
+      </c>
+      <c r="E178">
+        <v>12.1216139430431</v>
+      </c>
+      <c r="F178">
+        <v>17.052813608650901</v>
+      </c>
+      <c r="G178">
+        <v>14.0885362969229</v>
+      </c>
+      <c r="H178">
+        <v>8.4455258363931005</v>
       </c>
       <c r="I178" s="64" t="s">
         <v>164</v>
@@ -5309,19 +5362,46 @@
       <c r="B179">
         <v>224</v>
       </c>
-      <c r="C179">
-        <v>1.2459999999999999E-3</v>
-      </c>
-      <c r="D179" t="s">
-        <v>171</v>
+      <c r="C179" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179">
+        <v>1.2465816300111601E-3</v>
+      </c>
+      <c r="E179">
+        <v>3.79820862757327</v>
+      </c>
+      <c r="F179">
+        <v>7.1807943448157703</v>
+      </c>
+      <c r="G179">
+        <v>9.1721155359348607</v>
+      </c>
+      <c r="H179">
+        <v>6.7199438839471402</v>
       </c>
     </row>
     <row r="180" spans="2:9">
       <c r="B180">
         <v>221</v>
       </c>
-      <c r="C180" s="40">
-        <v>1.2570000000000001E-3</v>
+      <c r="C180" t="s">
+        <v>31</v>
+      </c>
+      <c r="D180">
+        <v>1.2486142083966601E-3</v>
+      </c>
+      <c r="E180">
+        <v>11.999317101382401</v>
+      </c>
+      <c r="F180">
+        <v>16.718513671953701</v>
+      </c>
+      <c r="G180">
+        <v>14.098405112563199</v>
+      </c>
+      <c r="H180">
+        <v>8.3232289947323999</v>
       </c>
       <c r="I180" s="64" t="s">
         <v>165</v>
@@ -5331,11 +5411,23 @@
       <c r="B181">
         <v>225</v>
       </c>
-      <c r="C181" s="40">
-        <v>1.248E-3</v>
-      </c>
-      <c r="D181" t="s">
-        <v>171</v>
+      <c r="C181" t="s">
+        <v>32</v>
+      </c>
+      <c r="D181">
+        <v>1.2486142083966601E-3</v>
+      </c>
+      <c r="E181">
+        <v>3.7207570340310201</v>
+      </c>
+      <c r="F181">
+        <v>7.2116517800519899</v>
+      </c>
+      <c r="G181">
+        <v>9.0161099358174006</v>
+      </c>
+      <c r="H181">
+        <v>6.64249229040482</v>
       </c>
     </row>
     <row r="182" spans="2:9">
@@ -5349,12 +5441,17 @@
         <v>166</v>
       </c>
     </row>
+    <row r="183" spans="2:9">
+      <c r="C183" t="s">
+        <v>172</v>
+      </c>
+    </row>
     <row r="184" spans="2:9">
       <c r="B184">
         <v>222</v>
       </c>
       <c r="C184" t="s">
-        <v>55</v>
+        <v>171</v>
       </c>
       <c r="I184" t="s">
         <v>167</v>
@@ -8646,7 +8743,7 @@
   <dimension ref="B1:M35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>